<commit_message>
Revision de carpeta y actividades
</commit_message>
<xml_diff>
--- a/Primera Entrega/Clase 8- Memoria/Alumnos/TomasJesusDelValle_DeLaPena/Clase 8 Memorias Juegos.xlsx
+++ b/Primera Entrega/Clase 8- Memoria/Alumnos/TomasJesusDelValle_DeLaPena/Clase 8 Memorias Juegos.xlsx
@@ -1,17 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\Mochila_0522C6\Primera Entrega\Clase 8- Memoria\Alumnos\TomasJesusDelValle_DeLaPena\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40CBF15-B0E2-42F4-A395-60FDD89F95A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>TAMAMO</t>
   </si>
@@ -62,26 +83,30 @@
   </si>
   <si>
     <t>PES</t>
+  </si>
+  <si>
+    <t>Conclusion Pueden Instalarse 11 Juegos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
@@ -91,40 +116,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -314,23 +344,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="23.13"/>
+    <col min="4" max="4" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -346,10 +381,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -358,17 +393,17 @@
         <v>5</v>
       </c>
       <c r="F2" s="1">
-        <v>6144.0</v>
+        <v>6144</v>
       </c>
       <c r="G2" s="3">
         <f>F2-F4</f>
-        <v>1132.6</v>
+        <v>1132.6000000000004</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>49.8</v>
@@ -383,7 +418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>78.2</v>
@@ -396,16 +431,16 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B:B)</f>
-        <v>5011.4</v>
+        <v>5011.3999999999996</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -414,10 +449,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
-        <v>363.0</v>
+        <v>363</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -426,10 +461,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
-        <v>663.0</v>
+        <v>663</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -438,10 +473,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
-        <v>682.0</v>
+        <v>682</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -450,7 +485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>491.4</v>
@@ -462,10 +497,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
-        <v>752.0</v>
+        <v>752</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -474,10 +509,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
-        <v>834.0</v>
+        <v>834</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -486,10 +521,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
-        <v>975.0</v>
+        <v>975</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
@@ -498,7 +533,12 @@
         <v>16</v>
       </c>
     </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>